<commit_message>
Update công nợ + nhập hàng
</commit_message>
<xml_diff>
--- a/TDStore/Công Nợ.xlsx
+++ b/TDStore/Công Nợ.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\01.GIT\04.Private\TDStore\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\06.TDStore\04.Private\TDStore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB0D5667-6D4F-4DD2-B17A-73E905C9A34F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C830033-F29F-4639-8086-4E411C675F42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B4E93AD0-FCAE-45CC-9919-8B3F8197C095}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Hiền Thỏ" sheetId="2" r:id="rId2"/>
     <sheet name="Quân" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -523,7 +523,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update công nợ Hảo
</commit_message>
<xml_diff>
--- a/TDStore/Công Nợ.xlsx
+++ b/TDStore/Công Nợ.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\06.TDStore\04.Private\TDStore\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\04.Private\TDStore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C830033-F29F-4639-8086-4E411C675F42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E2EE70A-D7B6-4237-8136-04B7B846B09C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B4E93AD0-FCAE-45CC-9919-8B3F8197C095}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Hiền Thỏ" sheetId="2" r:id="rId2"/>
     <sheet name="Quân" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="16">
   <si>
     <t>Máy</t>
   </si>
@@ -72,12 +72,6 @@
   </si>
   <si>
     <t>Tổng</t>
-  </si>
-  <si>
-    <t>14/07/23</t>
-  </si>
-  <si>
-    <t>Dell latitude 5400</t>
   </si>
   <si>
     <t>19/08/2023</t>
@@ -523,7 +517,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection sqref="A1:J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,7 +621,7 @@
         <v>2000000</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" ref="I4:I7" si="0">B4-C4-E4</f>
@@ -647,12 +641,18 @@
       <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E5" s="1">
+        <v>1600000</v>
+      </c>
+      <c r="F5" s="4">
+        <v>45178</v>
+      </c>
       <c r="I5" s="1">
-        <f t="shared" si="0"/>
-        <v>4500000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <f>B5-C5-E5</f>
+        <v>2900000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -680,27 +680,12 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="1">
-        <v>5000000</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1600000</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="1">
-        <f t="shared" si="0"/>
-        <v>3400000</v>
-      </c>
+      <c r="I7" s="1"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I9" s="1">
         <f>SUM(I3:I7)</f>
-        <v>9700000</v>
+        <v>4700000</v>
       </c>
       <c r="J9" t="s">
         <v>14</v>

</xml_diff>